<commit_message>
improvement; * added info about OLED Arduino library              * added todo for schematic              * added todo for mechanics              * modified code for testing a bit new feature; * added part list
</commit_message>
<xml_diff>
--- a/Materialliste.xlsx
+++ b/Materialliste.xlsx
@@ -19,64 +19,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Arduino Uno</t>
-  </si>
-  <si>
-    <t>A4988</t>
-  </si>
-  <si>
-    <t>Steper Motor</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>Lichtschranke</t>
-  </si>
-  <si>
-    <t>Kabel Lichtschranke</t>
-  </si>
-  <si>
-    <t>Werkstatt</t>
-  </si>
-  <si>
-    <t>Schlitten PTFE</t>
-  </si>
-  <si>
-    <t>Anschlag Al (besser SS?)</t>
-  </si>
-  <si>
-    <t>Endplatte Al</t>
-  </si>
-  <si>
-    <t>Best-Nr.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Preis</t>
   </si>
   <si>
-    <t>(Stellringe)</t>
-  </si>
-  <si>
-    <t>Mikorschalter</t>
-  </si>
-  <si>
     <t>Laden</t>
   </si>
   <si>
-    <t>Relais</t>
-  </si>
-  <si>
-    <t>PHYS Shop</t>
+    <t>Original Arduino Uno R3 (Atmega328) *RETAIL*</t>
+  </si>
+  <si>
+    <t>www.play-zone.ch</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>lager.phys.ethz.ch</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Art.-Nr.</t>
+  </si>
+  <si>
+    <t>3D-Druck</t>
+  </si>
+  <si>
+    <t>A4988 Stepper Driver Modul</t>
+  </si>
+  <si>
+    <t>bei www.distrelec.ch CHF 30.35 / bei www.3dware.ch CHF 4.20</t>
+  </si>
+  <si>
+    <t>OLED Modul 128 x 64 Pixel, I2C, Weiss, 0.96 inch, SSD1306</t>
+  </si>
+  <si>
+    <t>OLED Modul 1.3" / 128 x 64 Pixel, I2C, Weiss, SH1106</t>
+  </si>
+  <si>
+    <t>welcher? SSD1306 oder …</t>
+  </si>
+  <si>
+    <t>… SH1106? welchen habe ich hier? Siehe auch https://forum.arduino.cc/index.php?topic=256374.0</t>
+  </si>
+  <si>
+    <t>Betrieben mit 12V (mehr Drehmoment, weniger blockieren) - Kühlung??</t>
+  </si>
+  <si>
+    <t>Stepper Motor, 200 step, DC 8.64V, 0.24A</t>
+  </si>
+  <si>
+    <t>FIRST-Lab</t>
+  </si>
+  <si>
+    <t>Profil-System (Item, Kanya, etc.) Profil 40 x 40 x 100 mm</t>
+  </si>
+  <si>
+    <t>Leuchtenklemmen, 6mm2</t>
+  </si>
+  <si>
+    <t>(ca. 25.00)</t>
+  </si>
+  <si>
+    <t>Spindel M5 x 100mm, 0.8mm/Umdrehung</t>
+  </si>
+  <si>
+    <t>Gabellichtschranke, PM-T64, Panasonic</t>
+  </si>
+  <si>
+    <t>www.distrelec.ch</t>
+  </si>
+  <si>
+    <t>300-38-924</t>
+  </si>
+  <si>
+    <t>Konfektioniertes Kabel, 2 m, 3.7 mm, 0.2 mm² 4-Core, CN-14A-C2, Panasonic</t>
+  </si>
+  <si>
+    <t>300-38-891</t>
+  </si>
+  <si>
+    <t>Stellringe, 3, 7, M2</t>
+  </si>
+  <si>
+    <t>Miniatur-Mikroschalter, mit Hebel</t>
+  </si>
+  <si>
+    <t>Relais, TX2-5V, Panasonic</t>
+  </si>
+  <si>
+    <t>137-10-935</t>
+  </si>
+  <si>
+    <t>Bronze-Buchse M5</t>
+  </si>
+  <si>
+    <t>besser SS? wegen Verschleiss…?</t>
+  </si>
+  <si>
+    <t>(Lehr-)Werkstatt</t>
+  </si>
+  <si>
+    <t>Schlitten PTFE: "Catia\Saegeblatt_Schlitten.pdf"</t>
+  </si>
+  <si>
+    <t>Anschlag Al: "Catia\Saegeblatt_Anschlag.pdf"</t>
+  </si>
+  <si>
+    <t>Endplatte Al: "Catia\Saegeblatt_Endplatte.pdf"</t>
+  </si>
+  <si>
+    <t>Kupplungen/Klaue/Nabenklemmung mit Passfedernut: https://de.misumi-ec.com/vona2/detail/110300125940/</t>
+  </si>
+  <si>
+    <t>Wellenkupplung: http://forums.reprap.org/read.php?246,280197</t>
+  </si>
+  <si>
+    <t>Kardan: https://de.aliexpress.com/item/5pcs-Cross-universal-joint-drive-shaft-axle-coupling-metal-connector-diy-toy-accessories-technology-model-parts/32827812832.html</t>
+  </si>
+  <si>
+    <t>Drehstarre Kupplung: http://shop.myhobby-cnc.de/bauteile/mechanische-bauteile/kleinteile/21/drehstarre-kupplung</t>
+  </si>
+  <si>
+    <t>ROTEX Kupplung KTR Rotex 28: http://www.maschinenteil24.de/Mechanik/Mechanische-Baugruppen/Kupplungen/Kupplung-KTR-Rotex-28.html</t>
+  </si>
+  <si>
+    <t>Starre Kupplungen: http://www.directindustry.de/industrie-hersteller/starre-kupplung-61105.html</t>
+  </si>
+  <si>
+    <t>Vermeidung von Kupplungsausfällen: http://deutsch.ruland.com/a_articles_avoid_coup_failure_de.asp</t>
+  </si>
+  <si>
+    <t>welche Kupplung?</t>
+  </si>
+  <si>
+    <t>Kostenstelle ist 2205, Vermerk "Wafersäge"</t>
+  </si>
+  <si>
+    <t>Verbindung Stepper Motor zu Profil-System, blau, H.J. Rusterholz</t>
+  </si>
+  <si>
+    <t>Was für System haben wir verwendet?</t>
+  </si>
+  <si>
+    <t>PVC-Schläuche, 2, 4</t>
+  </si>
+  <si>
+    <t>15 mm</t>
+  </si>
+  <si>
+    <t>Kühlkörper, Typ FK 214/SA CB, 15 K/W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,13 +186,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,8 +229,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -387,107 +523,400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>28.9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14.9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>30067.599999999999</v>
+      </c>
+      <c r="D13">
+        <v>1.79</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>20247.2</v>
+      </c>
+      <c r="D14">
+        <v>0.43</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F14" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>40001.1</v>
+      </c>
+      <c r="D15">
+        <v>0.37</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>30049.4</v>
+      </c>
+      <c r="D16">
+        <v>0.64</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>18.36</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>3.51</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
+      <c r="C29">
         <v>30167.200000000001</v>
       </c>
-      <c r="D9">
+      <c r="D29">
         <v>8.74</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clean-up; * part list updated
</commit_message>
<xml_diff>
--- a/Materialliste.xlsx
+++ b/Materialliste.xlsx
@@ -178,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +196,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -229,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -243,6 +251,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -525,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,20 +851,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <v>3.51</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>